<commit_message>
Change document Review PT Docs
</commit_message>
<xml_diff>
--- a/Docs/Login.xlsx
+++ b/Docs/Login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Tai Lieu_Talent\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBF5626-DD29-44CB-8CA0-D590EC3B69CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E26AB58-5576-4534-9617-814DBD35ED5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>Tên hạng mục</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Nhớ mật khẩu</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -233,13 +230,51 @@
   </si>
   <si>
     <t>Email đã nhập không khớp với bất kỳ tài khoản nào!</t>
+  </si>
+  <si>
+    <t>5. Checkbox "Duy trì đăng nhập"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.1 . Có check </t>
+  </si>
+  <si>
+    <t>User sẽ duy trì trạng thái Login ( nếu không hoạt động trong 120p)</t>
+  </si>
+  <si>
+    <t>5.2 Không check</t>
+  </si>
+  <si>
+    <t>User sẽ bị logout nếu không hoạt động trong 120p</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nhớ mật khẩu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Duy trì đăng nhập</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +309,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -358,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -381,6 +424,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,15 +442,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -757,19 +802,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F5A53C-4A19-44A9-A25E-AFE844643C7E}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -787,7 +836,7 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -817,7 +866,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -834,29 +883,33 @@
         <v>9</v>
       </c>
       <c r="E5" s="1"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+      <c r="G6" s="19">
+        <v>44053</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -866,7 +919,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -879,10 +932,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -944,8 +997,8 @@
   </sheetPr>
   <dimension ref="A2:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,22 +1022,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -992,7 +1045,7 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="5"/>
@@ -1002,47 +1055,47 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="7"/>
-      <c r="I3" s="12" t="s">
-        <v>23</v>
+      <c r="I3" s="15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="16" t="s">
-        <v>19</v>
+      <c r="E4" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="13"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>67</v>
+        <v>18</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="13"/>
-      <c r="K5" s="17">
+      <c r="I5" s="16"/>
+      <c r="K5" s="14">
         <v>44112</v>
       </c>
     </row>
@@ -1050,19 +1103,19 @@
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="15" t="s">
-        <v>66</v>
+      <c r="G6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="H6" s="7"/>
-      <c r="I6" s="13"/>
-      <c r="K6" s="17">
+      <c r="I6" s="16"/>
+      <c r="K6" s="14">
         <v>44112</v>
       </c>
     </row>
@@ -1070,46 +1123,46 @@
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="15" t="s">
-        <v>25</v>
+      <c r="G7" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="13"/>
-      <c r="K7" s="17">
+      <c r="I7" s="16"/>
+      <c r="K7" s="14">
         <v>44112</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="13"/>
+        <v>58</v>
+      </c>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5">
         <v>50</v>
@@ -1117,10 +1170,10 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="7"/>
-      <c r="I9" s="14"/>
+      <c r="I9" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1138,10 +1191,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE144D9B-7E26-42AA-8E39-554455F95353}">
-  <dimension ref="A1:E40"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,100 +1206,101 @@
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1252,7 +1309,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -1263,78 +1320,139 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="H42" s="19">
+        <v>44112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>